<commit_message>
Update Pick Place for medusa-ai-integrated.xlsx
</commit_message>
<xml_diff>
--- a/altium/Medusa-AI-integrated-charger/Project Outputs for Medusa-AI-integrated-charger/Pick Place for medusa-ai-integrated.xlsx
+++ b/altium/Medusa-AI-integrated-charger/Project Outputs for Medusa-AI-integrated-charger/Pick Place for medusa-ai-integrated.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\w\medusa-AI\altium\Medusa-AI-integrated-charger\Project Outputs for Medusa-AI-integrated-charger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1257A0F3-E083-4D10-B972-CDD5CFC07397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DE86F6-F290-4155-81D3-9D5C06578B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33570" yWindow="240" windowWidth="21600" windowHeight="14925"/>
+    <workbookView xWindow="33570" yWindow="240" windowWidth="21600" windowHeight="14925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pick Place for medusa-ai-integr" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="172">
   <si>
     <t>Designator</t>
   </si>
@@ -274,12 +274,6 @@
     <t>Iridium9603</t>
   </si>
   <si>
-    <t>P3</t>
-  </si>
-  <si>
-    <t>Teensy3.x</t>
-  </si>
-  <si>
     <t>P2</t>
   </si>
   <si>
@@ -289,27 +283,6 @@
     <t>microSD_Molex_hinged</t>
   </si>
   <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>Header 20X2</t>
-  </si>
-  <si>
-    <t>HDR2X20</t>
-  </si>
-  <si>
-    <t>Header, 20-Pin, Dual row</t>
-  </si>
-  <si>
-    <t>MP1</t>
-  </si>
-  <si>
-    <t>MS223-10F</t>
-  </si>
-  <si>
-    <t>RF Shield</t>
-  </si>
-  <si>
     <t>L3</t>
   </si>
   <si>
@@ -560,12 +533,15 @@
   </si>
   <si>
     <t>1nF 50V</t>
+  </si>
+  <si>
+    <t>0.47uH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1402,11 +1378,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K88"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:XFD57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,10 +1424,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C2" s="1">
         <v>402</v>
@@ -1477,7 +1453,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>17</v>
@@ -1506,10 +1482,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C4" s="1">
         <v>402</v>
@@ -1535,10 +1511,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C5" s="1">
         <v>402</v>
@@ -1564,10 +1540,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C6" s="1">
         <v>402</v>
@@ -1593,10 +1569,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C7" s="1">
         <v>402</v>
@@ -1622,7 +1598,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>17</v>
@@ -1651,10 +1627,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C9" s="1">
         <v>402</v>
@@ -1680,10 +1656,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C10" s="1">
         <v>402</v>
@@ -1709,10 +1685,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C11" s="1">
         <v>402</v>
@@ -1738,10 +1714,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C12" s="1">
         <v>402</v>
@@ -1767,10 +1743,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>18</v>
@@ -1793,10 +1769,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C14" s="1">
         <v>402</v>
@@ -1822,10 +1798,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C15" s="1">
         <v>402</v>
@@ -1851,10 +1827,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C16" s="1">
         <v>402</v>
@@ -1880,10 +1856,10 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C17" s="1">
         <v>402</v>
@@ -1909,10 +1885,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C18" s="1">
         <v>402</v>
@@ -1938,10 +1914,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C19" s="1">
         <v>402</v>
@@ -1967,10 +1943,10 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C20" s="1">
         <v>402</v>
@@ -1996,10 +1972,10 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C21" s="1">
         <v>402</v>
@@ -2025,10 +2001,10 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C22" s="1">
         <v>402</v>
@@ -2054,10 +2030,10 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C23" s="1">
         <v>402</v>
@@ -2083,10 +2059,10 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C24" s="1">
         <v>402</v>
@@ -2112,10 +2088,10 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C25" s="1">
         <v>402</v>
@@ -2225,13 +2201,13 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D29" s="1">
         <v>-81.596000000000004</v>
@@ -2240,7 +2216,7 @@
         <v>55.439</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="I29">
         <v>81.596000000000004</v>
@@ -2254,10 +2230,10 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C30" s="1">
         <v>402</v>
@@ -2283,10 +2259,10 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C31" s="1">
         <v>603</v>
@@ -2312,10 +2288,10 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C32" s="1">
         <v>603</v>
@@ -2341,10 +2317,10 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C33" s="1">
         <v>1206</v>
@@ -2370,10 +2346,10 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C34" s="1">
         <v>402</v>
@@ -2399,13 +2375,13 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D35" s="1">
         <v>-35.494999999999997</v>
@@ -2414,7 +2390,7 @@
         <v>13.148</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="I35">
         <v>35.494999999999997</v>
@@ -2428,13 +2404,13 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D36" s="1">
         <v>-44.512</v>
@@ -2443,7 +2419,7 @@
         <v>13.275</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="I36">
         <v>44.512</v>
@@ -2457,10 +2433,10 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C37" s="1">
         <v>603</v>
@@ -2472,7 +2448,7 @@
         <v>9.7189999999999994</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="I37">
         <v>19.239000000000001</v>
@@ -2486,10 +2462,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C38" s="1">
         <v>805</v>
@@ -2515,10 +2491,10 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C39" s="1">
         <v>1206</v>
@@ -2544,10 +2520,10 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C40" s="1">
         <v>402</v>
@@ -2573,10 +2549,10 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C41" s="1">
         <v>805</v>
@@ -2602,10 +2578,10 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C42" s="1">
         <v>402</v>
@@ -2631,7 +2607,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>17</v>
@@ -2660,10 +2636,10 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C44" s="1">
         <v>402</v>
@@ -2689,10 +2665,10 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C45" s="1">
         <v>402</v>
@@ -2718,10 +2694,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C46" s="1">
         <v>402</v>
@@ -2747,13 +2723,13 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D47" s="1">
         <v>-23.303000000000001</v>
@@ -2773,13 +2749,13 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D48" s="1">
         <v>-14.794</v>
@@ -2799,13 +2775,13 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D49" s="1">
         <v>-67.563999999999993</v>
@@ -2912,13 +2888,13 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D53" s="1">
         <v>-90.075999999999993</v>
@@ -2927,7 +2903,7 @@
         <v>31.323</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="I53">
         <v>90.075999999999993</v>
@@ -2941,13 +2917,13 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>100</v>
+        <v>171</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D54" s="1">
         <v>-40.231999999999999</v>
@@ -2967,13 +2943,13 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D55" s="1">
         <v>-70.866</v>
@@ -2993,83 +2969,80 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D56" s="1">
-        <v>7.3040000000000003</v>
+        <v>-74.203999999999994</v>
       </c>
       <c r="E56" s="1">
-        <v>163.77000000000001</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>95</v>
+        <v>101.768</v>
       </c>
       <c r="I56">
-        <v>-7.3040000000000003</v>
+        <v>74.203999999999994</v>
       </c>
       <c r="J56">
-        <v>-163.77000000000001</v>
+        <v>-101.768</v>
       </c>
       <c r="K56">
-        <v>180</v>
+        <v>270</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D57" s="1">
-        <v>-58.631</v>
+        <v>-144.06700000000001</v>
       </c>
       <c r="E57" s="1">
-        <v>95.278000000000006</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>92</v>
+        <v>106.518</v>
       </c>
       <c r="I57">
-        <v>58.631</v>
+        <v>144.06700000000001</v>
       </c>
       <c r="J57">
-        <v>-95.278000000000006</v>
+        <v>-106.518</v>
       </c>
       <c r="K57">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="D58" s="1">
-        <v>-74.203999999999994</v>
+        <v>-89.07</v>
       </c>
       <c r="E58" s="1">
-        <v>101.768</v>
+        <v>132.68700000000001</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="I58">
-        <v>74.203999999999994</v>
+        <v>89.07</v>
       </c>
       <c r="J58">
-        <v>-101.768</v>
+        <v>-132.68700000000001</v>
       </c>
       <c r="K58">
         <v>270</v>
@@ -3077,25 +3050,28 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="D59" s="1">
-        <v>-92.921000000000006</v>
+        <v>-59.182000000000002</v>
       </c>
       <c r="E59" s="1">
-        <v>105.438</v>
+        <v>10.032999999999999</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="I59">
-        <v>92.921000000000006</v>
+        <v>59.182000000000002</v>
       </c>
       <c r="J59">
-        <v>-105.438</v>
+        <v>-10.032999999999999</v>
       </c>
       <c r="K59">
         <v>180</v>
@@ -3103,25 +3079,28 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="D60" s="1">
-        <v>-144.06700000000001</v>
+        <v>-62.8</v>
       </c>
       <c r="E60" s="1">
-        <v>106.518</v>
+        <v>20.006</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="I60">
-        <v>144.06700000000001</v>
+        <v>62.8</v>
       </c>
       <c r="J60">
-        <v>-106.518</v>
+        <v>-20.006</v>
       </c>
       <c r="K60">
         <v>180</v>
@@ -3129,28 +3108,28 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>80</v>
+        <v>161</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D61" s="1">
-        <v>-89.07</v>
+        <v>-58.801000000000002</v>
       </c>
       <c r="E61" s="1">
-        <v>132.68700000000001</v>
+        <v>19.05</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I61">
-        <v>89.07</v>
+        <v>58.801000000000002</v>
       </c>
       <c r="J61">
-        <v>-132.68700000000001</v>
+        <v>-19.05</v>
       </c>
       <c r="K61">
         <v>270</v>
@@ -3158,86 +3137,86 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>73</v>
+        <v>162</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D62" s="1">
-        <v>-59.182000000000002</v>
+        <v>-57.277000000000001</v>
       </c>
       <c r="E62" s="1">
-        <v>10.032999999999999</v>
+        <v>19.05</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I62">
-        <v>59.182000000000002</v>
+        <v>57.277000000000001</v>
       </c>
       <c r="J62">
-        <v>-10.032999999999999</v>
+        <v>-19.05</v>
       </c>
       <c r="K62">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="D63" s="1">
-        <v>-62.8</v>
+        <v>-55.753</v>
       </c>
       <c r="E63" s="1">
-        <v>20.006</v>
+        <v>19.05</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="I63">
-        <v>62.8</v>
+        <v>55.753</v>
       </c>
       <c r="J63">
-        <v>-20.006</v>
+        <v>-19.05</v>
       </c>
       <c r="K63">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>170</v>
+        <v>7</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D64" s="1">
-        <v>-58.801000000000002</v>
+        <v>-88.094999999999999</v>
       </c>
       <c r="E64" s="1">
-        <v>19.05</v>
+        <v>154.46</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I64">
-        <v>58.801000000000002</v>
+        <v>88.094999999999999</v>
       </c>
       <c r="J64">
-        <v>-19.05</v>
+        <v>-154.46</v>
       </c>
       <c r="K64">
         <v>270</v>
@@ -3245,28 +3224,28 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>171</v>
+        <v>79</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D65" s="1">
-        <v>-57.277000000000001</v>
+        <v>-91.228999999999999</v>
       </c>
       <c r="E65" s="1">
-        <v>19.05</v>
+        <v>132.68700000000001</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I65">
-        <v>57.277000000000001</v>
+        <v>91.228999999999999</v>
       </c>
       <c r="J65">
-        <v>-19.05</v>
+        <v>-132.68700000000001</v>
       </c>
       <c r="K65">
         <v>90</v>
@@ -3274,202 +3253,202 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D66" s="1">
-        <v>-55.753</v>
+        <v>-113.07299999999999</v>
       </c>
       <c r="E66" s="1">
-        <v>19.05</v>
+        <v>34.427999999999997</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I66">
-        <v>55.753</v>
+        <v>113.07299999999999</v>
       </c>
       <c r="J66">
-        <v>-19.05</v>
+        <v>-34.427999999999997</v>
       </c>
       <c r="K66">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D67" s="1">
-        <v>-88.094999999999999</v>
+        <v>-111.16800000000001</v>
       </c>
       <c r="E67" s="1">
-        <v>154.46</v>
+        <v>34.427999999999997</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I67">
-        <v>88.094999999999999</v>
+        <v>111.16800000000001</v>
       </c>
       <c r="J67">
-        <v>-154.46</v>
+        <v>-34.427999999999997</v>
       </c>
       <c r="K67">
-        <v>270</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>79</v>
+        <v>11</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D68" s="1">
-        <v>-91.228999999999999</v>
+        <v>-91.524000000000001</v>
       </c>
       <c r="E68" s="1">
-        <v>132.68700000000001</v>
+        <v>154.46</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I68">
-        <v>91.228999999999999</v>
+        <v>91.524000000000001</v>
       </c>
       <c r="J68">
-        <v>-132.68700000000001</v>
+        <v>-154.46</v>
       </c>
       <c r="K68">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>78</v>
+        <v>160</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D69" s="1">
-        <v>-113.07299999999999</v>
+        <v>-58.165999999999997</v>
       </c>
       <c r="E69" s="1">
-        <v>34.427999999999997</v>
+        <v>14.859</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I69">
-        <v>113.07299999999999</v>
+        <v>58.165999999999997</v>
       </c>
       <c r="J69">
-        <v>-34.427999999999997</v>
+        <v>-14.859</v>
       </c>
       <c r="K69">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>76</v>
+        <v>159</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D70" s="1">
-        <v>-111.16800000000001</v>
+        <v>-58.481999999999999</v>
       </c>
       <c r="E70" s="1">
-        <v>34.427999999999997</v>
+        <v>13.148</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I70">
-        <v>111.16800000000001</v>
+        <v>58.481999999999999</v>
       </c>
       <c r="J70">
-        <v>-34.427999999999997</v>
+        <v>-13.148</v>
       </c>
       <c r="K70">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>11</v>
+        <v>158</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D71" s="1">
-        <v>-91.524000000000001</v>
+        <v>-58.165999999999997</v>
       </c>
       <c r="E71" s="1">
-        <v>154.46</v>
+        <v>16.382999999999999</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I71">
-        <v>91.524000000000001</v>
+        <v>58.165999999999997</v>
       </c>
       <c r="J71">
-        <v>-154.46</v>
+        <v>-16.382999999999999</v>
       </c>
       <c r="K71">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D72" s="1">
-        <v>-58.165999999999997</v>
+        <v>-58.673999999999999</v>
       </c>
       <c r="E72" s="1">
-        <v>14.859</v>
+        <v>11.683999999999999</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I72">
-        <v>58.165999999999997</v>
+        <v>58.673999999999999</v>
       </c>
       <c r="J72">
-        <v>-14.859</v>
+        <v>-11.683999999999999</v>
       </c>
       <c r="K72">
         <v>0</v>
@@ -3477,57 +3456,57 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>168</v>
+        <v>61</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="D73" s="1">
-        <v>-58.481999999999999</v>
+        <v>-75.554000000000002</v>
       </c>
       <c r="E73" s="1">
-        <v>13.148</v>
+        <v>76.599999999999994</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="I73">
-        <v>58.481999999999999</v>
+        <v>75.554000000000002</v>
       </c>
       <c r="J73">
-        <v>-13.148</v>
+        <v>-76.599999999999994</v>
       </c>
       <c r="K73">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>167</v>
+        <v>39</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D74" s="1">
-        <v>-58.165999999999997</v>
+        <v>-73.314999999999998</v>
       </c>
       <c r="E74" s="1">
-        <v>16.382999999999999</v>
+        <v>115.178</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="I74">
-        <v>58.165999999999997</v>
+        <v>73.314999999999998</v>
       </c>
       <c r="J74">
-        <v>-16.382999999999999</v>
+        <v>-115.178</v>
       </c>
       <c r="K74">
         <v>0</v>
@@ -3535,86 +3514,83 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>166</v>
+        <v>19</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D75" s="1">
-        <v>-58.673999999999999</v>
+        <v>-129.62799999999999</v>
       </c>
       <c r="E75" s="1">
-        <v>11.683999999999999</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>10</v>
+        <v>144.67599999999999</v>
       </c>
       <c r="I75">
-        <v>58.673999999999999</v>
+        <v>129.62799999999999</v>
       </c>
       <c r="J75">
-        <v>-11.683999999999999</v>
+        <v>-144.67599999999999</v>
       </c>
       <c r="K75">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="D76" s="1">
-        <v>-75.554000000000002</v>
+        <v>-84.415999999999997</v>
       </c>
       <c r="E76" s="1">
-        <v>76.599999999999994</v>
+        <v>44.7</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="I76">
-        <v>75.554000000000002</v>
+        <v>84.415999999999997</v>
       </c>
       <c r="J76">
-        <v>-76.599999999999994</v>
+        <v>-44.7</v>
       </c>
       <c r="K76">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="D77" s="1">
-        <v>-73.314999999999998</v>
+        <v>-62.927</v>
       </c>
       <c r="E77" s="1">
-        <v>115.178</v>
+        <v>13.91</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="I77">
-        <v>73.314999999999998</v>
+        <v>62.927</v>
       </c>
       <c r="J77">
-        <v>-115.178</v>
+        <v>-13.91</v>
       </c>
       <c r="K77">
         <v>0</v>
@@ -3622,25 +3598,28 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="D78" s="1">
-        <v>-129.62799999999999</v>
+        <v>-124.417</v>
       </c>
       <c r="E78" s="1">
-        <v>144.67599999999999</v>
+        <v>49.891599999999997</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="I78">
-        <v>129.62799999999999</v>
+        <v>124.417</v>
       </c>
       <c r="J78">
-        <v>-144.67599999999999</v>
+        <v>-49.891599999999997</v>
       </c>
       <c r="K78">
         <v>180</v>
@@ -3648,28 +3627,28 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="D79" s="1">
-        <v>-84.415999999999997</v>
+        <v>-125.941</v>
       </c>
       <c r="E79" s="1">
-        <v>44.7</v>
+        <v>60.860999999999997</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="I79">
-        <v>84.415999999999997</v>
+        <v>125.941</v>
       </c>
       <c r="J79">
-        <v>-44.7</v>
+        <v>-60.860999999999997</v>
       </c>
       <c r="K79">
         <v>270</v>
@@ -3677,36 +3656,36 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="D80" s="1">
-        <v>-62.927</v>
+        <v>-115.934</v>
       </c>
       <c r="E80" s="1">
-        <v>13.91</v>
+        <v>78.637</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="I80">
-        <v>62.927</v>
+        <v>115.934</v>
       </c>
       <c r="J80">
-        <v>-13.91</v>
+        <v>-78.637</v>
       </c>
       <c r="K80">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>40</v>
@@ -3715,227 +3694,140 @@
         <v>41</v>
       </c>
       <c r="D81" s="1">
-        <v>-124.417</v>
+        <v>-122.744</v>
       </c>
       <c r="E81" s="1">
-        <v>49.891599999999997</v>
+        <v>72.710999999999999</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>42</v>
       </c>
       <c r="I81">
-        <v>124.417</v>
+        <v>122.744</v>
       </c>
       <c r="J81">
-        <v>-49.891599999999997</v>
+        <v>-72.710999999999999</v>
       </c>
       <c r="K81">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D82" s="1">
-        <v>-125.941</v>
+        <v>-117.4915</v>
       </c>
       <c r="E82" s="1">
-        <v>60.860999999999997</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>58</v>
+        <v>105.369</v>
       </c>
       <c r="I82">
-        <v>125.941</v>
+        <v>117.4915</v>
       </c>
       <c r="J82">
-        <v>-60.860999999999997</v>
+        <v>-105.369</v>
       </c>
       <c r="K82">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D83" s="1">
-        <v>-115.934</v>
+        <v>-117.321</v>
       </c>
       <c r="E83" s="1">
-        <v>78.637</v>
+        <v>112.08499999999999</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="I83">
-        <v>115.934</v>
+        <v>117.321</v>
       </c>
       <c r="J83">
-        <v>-78.637</v>
+        <v>-112.08499999999999</v>
       </c>
       <c r="K83">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D84" s="1">
-        <v>-122.744</v>
+        <v>-133.18</v>
       </c>
       <c r="E84" s="1">
-        <v>72.710999999999999</v>
+        <v>55.908000000000001</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="I84">
-        <v>122.744</v>
+        <v>133.18</v>
       </c>
       <c r="J84">
-        <v>-72.710999999999999</v>
+        <v>-55.908000000000001</v>
       </c>
       <c r="K84">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D85" s="1">
-        <v>-117.4915</v>
+        <v>-104.964</v>
       </c>
       <c r="E85" s="1">
-        <v>105.369</v>
+        <v>149.03399999999999</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="I85">
-        <v>117.4915</v>
+        <v>104.964</v>
       </c>
       <c r="J85">
-        <v>-105.369</v>
+        <v>-149.03399999999999</v>
       </c>
       <c r="K85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D86" s="1">
-        <v>-117.321</v>
-      </c>
-      <c r="E86" s="1">
-        <v>112.08499999999999</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I86">
-        <v>117.321</v>
-      </c>
-      <c r="J86">
-        <v>-112.08499999999999</v>
-      </c>
-      <c r="K86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D87" s="1">
-        <v>-133.18</v>
-      </c>
-      <c r="E87" s="1">
-        <v>55.908000000000001</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I87">
-        <v>133.18</v>
-      </c>
-      <c r="J87">
-        <v>-55.908000000000001</v>
-      </c>
-      <c r="K87">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D88" s="1">
-        <v>-104.964</v>
-      </c>
-      <c r="E88" s="1">
-        <v>149.03399999999999</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I88">
-        <v>104.964</v>
-      </c>
-      <c r="J88">
-        <v>-149.03399999999999</v>
-      </c>
-      <c r="K88">
         <v>270</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K90">
-    <sortCondition ref="A2:A90"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K87">
+    <sortCondition ref="A2:A87"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>